<commit_message>
DEV-11741: added a corporate bond
</commit_message>
<xml_diff>
--- a/examples/use-cases/orders-management/data/quotes.xlsx
+++ b/examples/use-cases/orders-management/data/quotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimBarrass\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3259AA5-9766-4049-B056-7219A514EADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BEF10A-3508-4565-BE19-A0217F66773E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1098" yWindow="1098" windowWidth="17280" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5685" yWindow="-12630" windowWidth="17280" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftse-100-prices31-Jul-2020-31-A" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>imd_34634534</t>
+  </si>
+  <si>
+    <t>Anglian Water 40LV</t>
+  </si>
+  <si>
+    <t>Fixed Income</t>
+  </si>
+  <si>
+    <t>imd_13579246</t>
   </si>
 </sst>
 </file>
@@ -902,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -966,6 +975,26 @@
         <v>13</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>110.93</v>
+      </c>
+      <c r="G3">
+        <v>112.2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
DEV-11741: added a commodities order
</commit_message>
<xml_diff>
--- a/examples/use-cases/orders-management/data/quotes.xlsx
+++ b/examples/use-cases/orders-management/data/quotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimBarrass\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BEF10A-3508-4565-BE19-A0217F66773E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EEE0AF-28FE-43CA-B552-DDE7D86E90AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5685" yWindow="-12630" windowWidth="17280" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1398" windowWidth="17280" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftse-100-prices31-Jul-2020-31-A" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>date</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t>imd_13579246</t>
+  </si>
+  <si>
+    <t>ZIZ21</t>
+  </si>
+  <si>
+    <t>ICE Silver 5000oz Dec21</t>
+  </si>
+  <si>
+    <t>Commodities</t>
+  </si>
+  <si>
+    <t>imd_12457801</t>
   </si>
 </sst>
 </file>
@@ -911,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -995,6 +1007,29 @@
         <v>16</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4">
+        <v>24.3</v>
+      </c>
+      <c r="G4">
+        <v>25.4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
SE-2885: Update for recent API changes
Several changes made to update function parameters to current requirements.
Re-ordered cells to create data before reading.
Removed extra lines from input files.
</commit_message>
<xml_diff>
--- a/examples/use-cases/orders-management/data/quotes.xlsx
+++ b/examples/use-cases/orders-management/data/quotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimBarrass\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dandasaro/work/code/github/sample-notebooks/examples/use-cases/orders-management/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EEE0AF-28FE-43CA-B552-DDE7D86E90AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FE83A4-7E5D-684B-B7A9-4915C25F70E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1398" windowWidth="17280" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1480" yWindow="1400" windowWidth="17280" windowHeight="9460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftse-100-prices31-Jul-2020-31-A" sheetId="1" r:id="rId1"/>
@@ -926,16 +926,16 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.796875" customWidth="1"/>
-    <col min="5" max="5" width="21.34765625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -961,7 +961,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -978,16 +978,16 @@
         <v>8</v>
       </c>
       <c r="F2">
-        <v>960</v>
+        <v>147</v>
       </c>
       <c r="G2">
-        <v>961.5</v>
+        <v>149.75</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
SE:2885 updated with current syntax and reordered quotes import.  Updated data files.
</commit_message>
<xml_diff>
--- a/examples/use-cases/orders-management/data/quotes.xlsx
+++ b/examples/use-cases/orders-management/data/quotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dandasaro/work/code/github/sample-notebooks/examples/use-cases/orders-management/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FE83A4-7E5D-684B-B7A9-4915C25F70E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DE5BA3-5C84-334C-AC5D-537D3E7D26F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="1400" windowWidth="17280" windowHeight="9460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21060" yWindow="-19120" windowWidth="17280" windowHeight="9460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftse-100-prices31-Jul-2020-31-A" sheetId="1" r:id="rId1"/>
@@ -926,7 +926,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -978,10 +978,10 @@
         <v>8</v>
       </c>
       <c r="F2">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="G2">
-        <v>149.75</v>
+        <v>111.5</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
SE-2885: Add example of GetHoldingsWithOrders (#687)
</commit_message>
<xml_diff>
--- a/examples/use-cases/orders-management/data/quotes.xlsx
+++ b/examples/use-cases/orders-management/data/quotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimBarrass\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dandasaro/work/code/github/sample-notebooks/examples/use-cases/orders-management/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EEE0AF-28FE-43CA-B552-DDE7D86E90AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DE5BA3-5C84-334C-AC5D-537D3E7D26F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1398" windowWidth="17280" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21060" yWindow="-19120" windowWidth="17280" windowHeight="9460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ftse-100-prices31-Jul-2020-31-A" sheetId="1" r:id="rId1"/>
@@ -926,16 +926,16 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.796875" customWidth="1"/>
-    <col min="5" max="5" width="21.34765625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -961,7 +961,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -978,16 +978,16 @@
         <v>8</v>
       </c>
       <c r="F2">
-        <v>960</v>
+        <v>111</v>
       </c>
       <c r="G2">
-        <v>961.5</v>
+        <v>111.5</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>

</xml_diff>